<commit_message>
no_bolsista para nome e dt_nascimento para data_nascimento. Separador de decimal alterado de . para ,
</commit_message>
<xml_diff>
--- a/relatorio/templates/relatorio/msoffice/Termo_de_Compromisso_de_Bolsista_PRJ.xlsx
+++ b/relatorio/templates/relatorio/msoffice/Termo_de_Compromisso_de_Bolsista_PRJ.xlsx
@@ -1,17 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="EstaPasta_de_trabalho"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ane.nobrega\Desktop\ProjetosLocal\Projetos\01-Projetos de Pesquisa\Projeto de 2016\02 - GEPRO_MPOG_TDC_DIPLA_2016\Gestao do Projeto\09- Formularios\Bolsa Pesquisa\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659AE32D-FCF0-4F89-9EC9-4F29A7FA733B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="11610" yWindow="0" windowWidth="12435" windowHeight="10065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11610" yWindow="0" windowWidth="12435" windowHeight="10065"/>
   </bookViews>
   <sheets>
     <sheet name="Bolsista" sheetId="1" r:id="rId1"/>
@@ -19,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Bolsista!$A$1:$M$43</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="500">
   <si>
     <t>Valor Mensal</t>
   </si>
@@ -1351,9 +1345,6 @@
     <t>Pesquisador</t>
   </si>
   <si>
-    <t>Nome:</t>
-  </si>
-  <si>
     <t>Vinculo outras IES:</t>
   </si>
   <si>
@@ -1367,33 +1358,6 @@
   </si>
   <si>
     <t>Autorizo o pagamento da bolsa pelo prazo de sua vigência, desde que as folhas sejam atestadas mensalmente pelo Coordenador do Projeto</t>
-  </si>
-  <si>
-    <t>Telefone:</t>
-  </si>
-  <si>
-    <t>E-mail:</t>
-  </si>
-  <si>
-    <t>CPF:</t>
-  </si>
-  <si>
-    <t>RG:</t>
-  </si>
-  <si>
-    <t>Endereço:</t>
-  </si>
-  <si>
-    <t>Celular:</t>
-  </si>
-  <si>
-    <t>Cidade:</t>
-  </si>
-  <si>
-    <t>UF:</t>
-  </si>
-  <si>
-    <t>Data de nascimento:</t>
   </si>
   <si>
     <t>1. Identificação do Projeto</t>
@@ -1621,15 +1585,6 @@
       </rPr>
       <t>acima</t>
     </r>
-  </si>
-  <si>
-    <t>Banco:</t>
-  </si>
-  <si>
-    <t>Agência:</t>
-  </si>
-  <si>
-    <t>Conta Corrente:</t>
   </si>
   <si>
     <t>5. Informar à qual atividade do Projeto está vinculada a concessão desta bolsa</t>
@@ -1903,9 +1858,6 @@
     </r>
   </si>
   <si>
-    <t>Nome:Pesquisa Aplicada em Planejamento Estratégico, Gestão de Riscos Corporativos e Gestão da Informação Corporativa no âmbito das competências da Diretoria de Planejamento e Gestão do Ministério do Planejamento, Orçamento e Gestão (DIPLA/MP).</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1958,20 +1910,6 @@
   </si>
   <si>
     <r>
-      <t>Sigla:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>GEPRO_TED_MP_DIPLA_GESTAO DE RISCO_2016</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Coordenador do Projeto:</t>
     </r>
     <r>
@@ -2029,11 +1967,97 @@
   <si>
     <t>Bolsa de Pesquisa e de Estimulo à Inovação</t>
   </si>
+  <si>
+    <t>Nome: {{ bolsista.nome }}</t>
+  </si>
+  <si>
+    <t>CPF: {{ bolsista.cpf }}</t>
+  </si>
+  <si>
+    <t>RG: {{ bolsista.rg }} {{ bolsista.orgao_expedidor }} </t>
+  </si>
+  <si>
+    <t>Data de nascimento: {{ bolsista.data_nascimento }}</t>
+  </si>
+  <si>
+    <t>Endereço: {{ bolsista.endereco }}</t>
+  </si>
+  <si>
+    <t>Telefone: {{ bolsista.telefone }}</t>
+  </si>
+  <si>
+    <t>Celular: {{ bolsista.celular }}</t>
+  </si>
+  <si>
+    <t>E-mail: {{ bolsista.email }}</t>
+  </si>
+  <si>
+    <t>Cidade: {{ bolsista.cidade }}</t>
+  </si>
+  <si>
+    <t>UF: {{ bolsista.uf }}</t>
+  </si>
+  <si>
+    <t>Banco: {{ bolsista.get_banco_display }}</t>
+  </si>
+  <si>
+    <t>Agência: {{ bolsista.agencia }}</t>
+  </si>
+  <si>
+    <t>Conta Corrente: {{ bolsista.conta }}</t>
+  </si>
+  <si>
+    <t>{{ projeto.inicio_vigencia }}</t>
+  </si>
+  <si>
+    <t>{{ projeto.termino_vigencia }}</t>
+  </si>
+  <si>
+    <t>Nome: {{ projeto.nome }}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sigla: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>{{ projeto.sigla }}</t>
+    </r>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>{{ participante.inicio_vigencia }}</t>
+  </si>
+  <si>
+    <t>{{ participante.termino_vigencia }}</t>
+  </si>
+  <si>
+    <t>{{ participante.valor_mensal }}</t>
+  </si>
+  <si>
+    <t>{{ participante.periodo_total }}</t>
+  </si>
+  <si>
+    <t>{{ participante.horas_semanais }}</t>
+  </si>
+  <si>
+    <t>atividades___</t>
+  </si>
+  <si>
+    <t>tituloppi___</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="&quot;R$ &quot;#,##0.00_);\(&quot;R$ &quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
@@ -2581,20 +2605,372 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2672,358 +3048,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3115,7 +3139,7 @@
         <xdr:cNvPr id="20" name="Conector reto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3162,7 +3186,7 @@
         <xdr:cNvPr id="21" name="Conector reto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3209,7 +3233,7 @@
         <xdr:cNvPr id="22" name="Conector reto 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3256,7 +3280,7 @@
         <xdr:cNvPr id="12" name="Conector reto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3298,7 +3322,7 @@
         <xdr:cNvPr id="2" name="CaixaDeTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3361,7 +3385,7 @@
         <xdr:cNvPr id="28" name="Imagem 27" descr="DPI-preto.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3409,14 +3433,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3424,29 +3445,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -3496,14 +3494,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3511,29 +3506,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -3583,14 +3555,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3598,29 +3567,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -3669,14 +3615,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1061"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3684,29 +3627,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -3755,14 +3675,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1063"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3770,29 +3687,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -3841,14 +3735,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1066"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3856,29 +3747,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -3927,14 +3795,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1067"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3942,29 +3807,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -4013,14 +3855,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1068"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4028,29 +3867,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -4099,14 +3915,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1069"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4114,29 +3927,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -4185,14 +3975,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1070"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4200,29 +3987,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -4271,14 +4035,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1071"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4286,29 +4047,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -4685,12 +4423,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:AD339"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4722,21 +4460,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="118" t="s">
-        <v>466</v>
-      </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="120"/>
+      <c r="A1" s="108" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="110"/>
       <c r="O1" s="4"/>
       <c r="S1" s="9" t="s">
         <v>15</v>
@@ -4747,19 +4485,19 @@
       <c r="U1" s="11"/>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="121"/>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="123"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="113"/>
       <c r="O2" s="4"/>
       <c r="S2" s="12" t="s">
         <v>17</v>
@@ -4773,21 +4511,21 @@
       </c>
     </row>
     <row r="3" spans="1:24" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="124" t="s">
-        <v>482</v>
-      </c>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
-      <c r="F3" s="125"/>
-      <c r="G3" s="125"/>
-      <c r="H3" s="125"/>
-      <c r="I3" s="125"/>
-      <c r="J3" s="125"/>
-      <c r="K3" s="125"/>
-      <c r="L3" s="125"/>
-      <c r="M3" s="126"/>
+      <c r="A3" s="114" t="s">
+        <v>468</v>
+      </c>
+      <c r="B3" s="115"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="116"/>
       <c r="O3" s="4"/>
       <c r="S3" s="12" t="s">
         <v>19</v>
@@ -4801,21 +4539,21 @@
       </c>
     </row>
     <row r="4" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="137" t="s">
-        <v>454</v>
-      </c>
-      <c r="B4" s="138"/>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="138"/>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="138"/>
-      <c r="K4" s="138"/>
-      <c r="L4" s="138"/>
-      <c r="M4" s="139"/>
+      <c r="A4" s="127" t="s">
+        <v>444</v>
+      </c>
+      <c r="B4" s="128"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="128"/>
+      <c r="M4" s="129"/>
       <c r="O4" s="4"/>
       <c r="S4" s="12" t="s">
         <v>21</v>
@@ -4829,23 +4567,23 @@
       </c>
     </row>
     <row r="5" spans="1:24" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="132" t="s">
-        <v>481</v>
-      </c>
-      <c r="B5" s="133"/>
-      <c r="C5" s="133"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="133"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="127" t="s">
+      <c r="A5" s="122" t="s">
+        <v>490</v>
+      </c>
+      <c r="B5" s="123"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="127"/>
-      <c r="L5" s="128"/>
-      <c r="M5" s="129" t="s">
+      <c r="K5" s="117"/>
+      <c r="L5" s="118"/>
+      <c r="M5" s="119" t="s">
         <v>11</v>
       </c>
       <c r="O5" s="4"/>
@@ -4861,42 +4599,42 @@
       </c>
     </row>
     <row r="6" spans="1:24" s="1" customFormat="1" ht="0.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="135"/>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
+      <c r="A6" s="125"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
       <c r="I6" s="45"/>
       <c r="J6" s="36"/>
       <c r="K6" s="37"/>
       <c r="L6" s="38"/>
-      <c r="M6" s="129"/>
+      <c r="M6" s="119"/>
       <c r="O6" s="4"/>
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
       <c r="U6" s="11"/>
     </row>
     <row r="7" spans="1:24" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="145"/>
-      <c r="B7" s="146"/>
-      <c r="C7" s="146"/>
-      <c r="D7" s="146"/>
-      <c r="E7" s="146"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="146"/>
-      <c r="H7" s="146"/>
-      <c r="I7" s="147"/>
+      <c r="A7" s="135"/>
+      <c r="B7" s="136"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="136"/>
+      <c r="H7" s="136"/>
+      <c r="I7" s="137"/>
       <c r="J7" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="129" t="s">
+      <c r="K7" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="129"/>
-      <c r="M7" s="129"/>
+      <c r="L7" s="119"/>
+      <c r="M7" s="119"/>
       <c r="O7" s="4"/>
       <c r="S7" s="12">
         <v>237</v>
@@ -4910,26 +4648,26 @@
       </c>
     </row>
     <row r="8" spans="1:24" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="140" t="s">
-        <v>484</v>
-      </c>
-      <c r="B8" s="141"/>
-      <c r="C8" s="142"/>
-      <c r="D8" s="140" t="s">
-        <v>483</v>
-      </c>
-      <c r="E8" s="143"/>
-      <c r="F8" s="143"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="143"/>
-      <c r="I8" s="144"/>
-      <c r="J8" s="56">
-        <v>42510</v>
-      </c>
-      <c r="K8" s="130">
-        <v>44335</v>
-      </c>
-      <c r="L8" s="131"/>
+      <c r="A8" s="130" t="s">
+        <v>491</v>
+      </c>
+      <c r="B8" s="131"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="130" t="s">
+        <v>469</v>
+      </c>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
+      <c r="H8" s="133"/>
+      <c r="I8" s="134"/>
+      <c r="J8" s="56" t="s">
+        <v>488</v>
+      </c>
+      <c r="K8" s="120" t="s">
+        <v>489</v>
+      </c>
+      <c r="L8" s="121"/>
       <c r="M8" s="18"/>
       <c r="O8" s="4"/>
       <c r="S8" s="12">
@@ -4944,19 +4682,19 @@
       </c>
     </row>
     <row r="9" spans="1:24" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="93" t="s">
-        <v>485</v>
-      </c>
-      <c r="B9" s="94"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="95"/>
+      <c r="A9" s="105" t="s">
+        <v>470</v>
+      </c>
+      <c r="B9" s="147"/>
+      <c r="C9" s="147"/>
+      <c r="D9" s="147"/>
+      <c r="E9" s="147"/>
+      <c r="F9" s="147"/>
+      <c r="G9" s="147"/>
+      <c r="H9" s="147"/>
+      <c r="I9" s="148"/>
       <c r="J9" s="41" t="s">
-        <v>488</v>
+        <v>473</v>
       </c>
       <c r="K9" s="42"/>
       <c r="L9" s="42"/>
@@ -4975,7 +4713,7 @@
     </row>
     <row r="10" spans="1:24" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>
@@ -4985,12 +4723,12 @@
       <c r="G10" s="49"/>
       <c r="H10" s="49"/>
       <c r="I10" s="49"/>
-      <c r="J10" s="86" t="s">
-        <v>487</v>
-      </c>
-      <c r="K10" s="87"/>
-      <c r="L10" s="87"/>
-      <c r="M10" s="88"/>
+      <c r="J10" s="138" t="s">
+        <v>472</v>
+      </c>
+      <c r="K10" s="139"/>
+      <c r="L10" s="139"/>
+      <c r="M10" s="140"/>
       <c r="O10" s="4"/>
       <c r="S10" s="12">
         <v>477</v>
@@ -5004,21 +4742,21 @@
       </c>
     </row>
     <row r="11" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="174" t="s">
-        <v>455</v>
-      </c>
-      <c r="B11" s="175"/>
-      <c r="C11" s="175"/>
-      <c r="D11" s="175"/>
-      <c r="E11" s="175"/>
-      <c r="F11" s="175"/>
-      <c r="G11" s="175"/>
-      <c r="H11" s="175"/>
-      <c r="I11" s="175"/>
-      <c r="J11" s="175"/>
-      <c r="K11" s="175"/>
-      <c r="L11" s="175"/>
-      <c r="M11" s="176"/>
+      <c r="A11" s="57" t="s">
+        <v>445</v>
+      </c>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="59"/>
       <c r="O11" s="4"/>
       <c r="S11" s="14" t="s">
         <v>28</v>
@@ -5033,19 +4771,19 @@
       <c r="X11" s="19"/>
     </row>
     <row r="12" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="157" t="s">
-        <v>465</v>
-      </c>
-      <c r="B12" s="158"/>
-      <c r="C12" s="158"/>
-      <c r="D12" s="158"/>
-      <c r="E12" s="158"/>
-      <c r="F12" s="158"/>
-      <c r="G12" s="158"/>
-      <c r="H12" s="158"/>
-      <c r="I12" s="158"/>
+      <c r="A12" s="87" t="s">
+        <v>455</v>
+      </c>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="88"/>
       <c r="J12" s="47" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K12" s="46"/>
       <c r="L12" s="46"/>
@@ -5057,21 +4795,21 @@
       <c r="X12" s="19"/>
     </row>
     <row r="13" spans="1:24" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="190" t="s">
-        <v>441</v>
-      </c>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="110"/>
-      <c r="L13" s="110"/>
-      <c r="M13" s="111"/>
+      <c r="A13" s="73" t="s">
+        <v>440</v>
+      </c>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="74"/>
+      <c r="M13" s="75"/>
       <c r="O13" s="4"/>
       <c r="S13" s="14"/>
       <c r="T13" s="14"/>
@@ -5079,21 +4817,21 @@
       <c r="X13" s="19"/>
     </row>
     <row r="14" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="109" t="s">
-        <v>439</v>
-      </c>
-      <c r="B14" s="110"/>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
-      <c r="K14" s="110"/>
-      <c r="L14" s="110"/>
-      <c r="M14" s="111"/>
+      <c r="A14" s="98" t="s">
+        <v>475</v>
+      </c>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="75"/>
       <c r="O14" s="4"/>
       <c r="S14" s="14"/>
       <c r="T14" s="14"/>
@@ -5101,25 +4839,25 @@
       <c r="X14" s="19"/>
     </row>
     <row r="15" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="109" t="s">
-        <v>447</v>
-      </c>
-      <c r="B15" s="111"/>
-      <c r="C15" s="109" t="s">
-        <v>448</v>
-      </c>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
-      <c r="G15" s="110"/>
-      <c r="H15" s="109" t="s">
-        <v>453</v>
-      </c>
-      <c r="I15" s="110"/>
-      <c r="J15" s="110"/>
-      <c r="K15" s="110"/>
-      <c r="L15" s="110"/>
-      <c r="M15" s="111"/>
+      <c r="A15" s="98" t="s">
+        <v>476</v>
+      </c>
+      <c r="B15" s="75"/>
+      <c r="C15" s="98" t="s">
+        <v>477</v>
+      </c>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="98" t="s">
+        <v>478</v>
+      </c>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="75"/>
       <c r="O15" s="4"/>
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
@@ -5127,24 +4865,24 @@
       <c r="X15" s="19"/>
     </row>
     <row r="16" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="109" t="s">
-        <v>449</v>
-      </c>
-      <c r="B16" s="110"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="110"/>
-      <c r="G16" s="111"/>
-      <c r="H16" s="109" t="s">
-        <v>451</v>
-      </c>
-      <c r="I16" s="110"/>
-      <c r="J16" s="110"/>
-      <c r="K16" s="110"/>
-      <c r="L16" s="111"/>
+      <c r="A16" s="98" t="s">
+        <v>479</v>
+      </c>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="98" t="s">
+        <v>483</v>
+      </c>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="75"/>
       <c r="M16" s="44" t="s">
-        <v>452</v>
+        <v>484</v>
       </c>
       <c r="O16" s="4"/>
       <c r="S16" s="14" t="s">
@@ -5159,25 +4897,25 @@
       </c>
     </row>
     <row r="17" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="191" t="s">
-        <v>445</v>
-      </c>
-      <c r="B17" s="192"/>
-      <c r="C17" s="178" t="s">
-        <v>450</v>
-      </c>
-      <c r="D17" s="179"/>
-      <c r="E17" s="179"/>
-      <c r="F17" s="179"/>
-      <c r="G17" s="180"/>
-      <c r="H17" s="93" t="s">
-        <v>446</v>
-      </c>
-      <c r="I17" s="172"/>
-      <c r="J17" s="172"/>
-      <c r="K17" s="172"/>
-      <c r="L17" s="172"/>
-      <c r="M17" s="173"/>
+      <c r="A17" s="76" t="s">
+        <v>480</v>
+      </c>
+      <c r="B17" s="77"/>
+      <c r="C17" s="61" t="s">
+        <v>481</v>
+      </c>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="105" t="s">
+        <v>482</v>
+      </c>
+      <c r="I17" s="106"/>
+      <c r="J17" s="106"/>
+      <c r="K17" s="106"/>
+      <c r="L17" s="106"/>
+      <c r="M17" s="107"/>
       <c r="O17" s="4"/>
       <c r="S17" s="14" t="s">
         <v>32</v>
@@ -5191,21 +4929,21 @@
       </c>
     </row>
     <row r="18" spans="1:21" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="187" t="s">
-        <v>456</v>
-      </c>
-      <c r="B18" s="188"/>
-      <c r="C18" s="188"/>
-      <c r="D18" s="188"/>
-      <c r="E18" s="188"/>
-      <c r="F18" s="188"/>
-      <c r="G18" s="188"/>
-      <c r="H18" s="188"/>
-      <c r="I18" s="188"/>
-      <c r="J18" s="188"/>
-      <c r="K18" s="188"/>
-      <c r="L18" s="188"/>
-      <c r="M18" s="189"/>
+      <c r="A18" s="70" t="s">
+        <v>446</v>
+      </c>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="71"/>
+      <c r="M18" s="72"/>
       <c r="O18" s="21"/>
       <c r="P18" s="21"/>
       <c r="Q18" s="21"/>
@@ -5222,25 +4960,25 @@
       </c>
     </row>
     <row r="19" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="181" t="s">
-        <v>471</v>
-      </c>
-      <c r="B19" s="182"/>
-      <c r="C19" s="182"/>
-      <c r="D19" s="182"/>
-      <c r="E19" s="182"/>
-      <c r="F19" s="182"/>
-      <c r="G19" s="183"/>
-      <c r="H19" s="181" t="s">
-        <v>472</v>
-      </c>
-      <c r="I19" s="182"/>
-      <c r="J19" s="183"/>
-      <c r="K19" s="186" t="s">
-        <v>473</v>
-      </c>
-      <c r="L19" s="186"/>
-      <c r="M19" s="186"/>
+      <c r="A19" s="64" t="s">
+        <v>485</v>
+      </c>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="64" t="s">
+        <v>486</v>
+      </c>
+      <c r="I19" s="65"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="69" t="s">
+        <v>487</v>
+      </c>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -5250,21 +4988,21 @@
       <c r="U19" s="11"/>
     </row>
     <row r="20" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="174" t="s">
-        <v>457</v>
-      </c>
-      <c r="B20" s="184"/>
-      <c r="C20" s="184"/>
-      <c r="D20" s="184"/>
-      <c r="E20" s="184"/>
-      <c r="F20" s="184"/>
-      <c r="G20" s="184"/>
-      <c r="H20" s="184"/>
-      <c r="I20" s="184"/>
-      <c r="J20" s="184"/>
-      <c r="K20" s="184"/>
-      <c r="L20" s="184"/>
-      <c r="M20" s="185"/>
+      <c r="A20" s="57" t="s">
+        <v>447</v>
+      </c>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="68"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
@@ -5282,26 +5020,26 @@
     </row>
     <row r="21" spans="1:21" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B21" s="29"/>
-      <c r="C21" s="115" t="s">
-        <v>463</v>
-      </c>
-      <c r="D21" s="116"/>
-      <c r="E21" s="116"/>
-      <c r="F21" s="116"/>
-      <c r="G21" s="117"/>
-      <c r="H21" s="112" t="s">
+      <c r="C21" s="163" t="s">
+        <v>453</v>
+      </c>
+      <c r="D21" s="164"/>
+      <c r="E21" s="164"/>
+      <c r="F21" s="164"/>
+      <c r="G21" s="165"/>
+      <c r="H21" s="160" t="s">
         <v>427</v>
       </c>
-      <c r="I21" s="113"/>
-      <c r="J21" s="114"/>
-      <c r="K21" s="177" t="s">
+      <c r="I21" s="161"/>
+      <c r="J21" s="162"/>
+      <c r="K21" s="60" t="s">
         <v>423</v>
       </c>
-      <c r="L21" s="177"/>
-      <c r="M21" s="177"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
       <c r="S21" s="14" t="s">
         <v>38</v>
       </c>
@@ -5314,25 +5052,29 @@
       </c>
     </row>
     <row r="22" spans="1:21" s="21" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="63" t="s">
-        <v>489</v>
-      </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="151" t="s">
+      <c r="A22" s="170" t="s">
+        <v>474</v>
+      </c>
+      <c r="B22" s="171"/>
+      <c r="C22" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="152"/>
-      <c r="E22" s="151" t="s">
+      <c r="D22" s="82"/>
+      <c r="E22" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="155"/>
-      <c r="G22" s="152"/>
-      <c r="H22" s="166"/>
-      <c r="I22" s="167"/>
-      <c r="J22" s="168"/>
-      <c r="K22" s="169"/>
-      <c r="L22" s="170"/>
-      <c r="M22" s="171"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="99" t="s">
+        <v>496</v>
+      </c>
+      <c r="I22" s="100"/>
+      <c r="J22" s="101"/>
+      <c r="K22" s="102" t="s">
+        <v>497</v>
+      </c>
+      <c r="L22" s="103"/>
+      <c r="M22" s="104"/>
       <c r="S22" s="23" t="s">
         <v>40</v>
       </c>
@@ -5351,21 +5093,21 @@
       <c r="B23" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="153"/>
-      <c r="D23" s="154"/>
-      <c r="E23" s="153"/>
-      <c r="F23" s="156"/>
-      <c r="G23" s="154"/>
-      <c r="H23" s="159" t="s">
+      <c r="C23" s="83"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="I23" s="160"/>
-      <c r="J23" s="161"/>
-      <c r="K23" s="162" t="s">
+      <c r="I23" s="90"/>
+      <c r="J23" s="91"/>
+      <c r="K23" s="92" t="s">
         <v>425</v>
       </c>
-      <c r="L23" s="162"/>
-      <c r="M23" s="162"/>
+      <c r="L23" s="92"/>
+      <c r="M23" s="92"/>
       <c r="O23" s="4"/>
       <c r="S23" s="14" t="s">
         <v>42</v>
@@ -5379,22 +5121,32 @@
       </c>
     </row>
     <row r="24" spans="1:21" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="103"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="104"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="99"/>
-      <c r="I24" s="100"/>
-      <c r="J24" s="101"/>
-      <c r="K24" s="102">
+      <c r="A24" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>492</v>
+      </c>
+      <c r="C24" s="96" t="s">
+        <v>493</v>
+      </c>
+      <c r="D24" s="97"/>
+      <c r="E24" s="96" t="s">
+        <v>494</v>
+      </c>
+      <c r="F24" s="156"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="152" t="s">
+        <v>495</v>
+      </c>
+      <c r="I24" s="153"/>
+      <c r="J24" s="154"/>
+      <c r="K24" s="155" t="e">
         <f>H24*H22</f>
-        <v>0</v>
-      </c>
-      <c r="L24" s="102"/>
-      <c r="M24" s="102"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L24" s="155"/>
+      <c r="M24" s="155"/>
       <c r="O24" s="4"/>
       <c r="S24" s="14" t="s">
         <v>44</v>
@@ -5408,21 +5160,21 @@
       </c>
     </row>
     <row r="25" spans="1:21" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="163" t="s">
-        <v>468</v>
-      </c>
-      <c r="B25" s="164"/>
-      <c r="C25" s="164"/>
-      <c r="D25" s="164"/>
-      <c r="E25" s="164"/>
-      <c r="F25" s="164"/>
-      <c r="G25" s="164"/>
-      <c r="H25" s="164"/>
-      <c r="I25" s="164"/>
-      <c r="J25" s="164"/>
-      <c r="K25" s="164"/>
-      <c r="L25" s="164"/>
-      <c r="M25" s="165"/>
+      <c r="A25" s="93" t="s">
+        <v>458</v>
+      </c>
+      <c r="B25" s="94"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="94"/>
+      <c r="G25" s="94"/>
+      <c r="H25" s="94"/>
+      <c r="I25" s="94"/>
+      <c r="J25" s="94"/>
+      <c r="K25" s="94"/>
+      <c r="L25" s="94"/>
+      <c r="M25" s="95"/>
       <c r="O25" s="4"/>
       <c r="S25" s="14" t="s">
         <v>46</v>
@@ -5436,21 +5188,21 @@
       </c>
     </row>
     <row r="26" spans="1:21" s="21" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="106" t="s">
-        <v>474</v>
-      </c>
-      <c r="B26" s="107"/>
-      <c r="C26" s="107"/>
-      <c r="D26" s="107"/>
-      <c r="E26" s="107"/>
-      <c r="F26" s="107"/>
-      <c r="G26" s="107"/>
-      <c r="H26" s="107"/>
-      <c r="I26" s="107"/>
-      <c r="J26" s="107"/>
-      <c r="K26" s="107"/>
-      <c r="L26" s="107"/>
-      <c r="M26" s="108"/>
+      <c r="A26" s="157" t="s">
+        <v>461</v>
+      </c>
+      <c r="B26" s="158"/>
+      <c r="C26" s="158"/>
+      <c r="D26" s="158"/>
+      <c r="E26" s="158"/>
+      <c r="F26" s="158"/>
+      <c r="G26" s="158"/>
+      <c r="H26" s="158"/>
+      <c r="I26" s="158"/>
+      <c r="J26" s="158"/>
+      <c r="K26" s="158"/>
+      <c r="L26" s="158"/>
+      <c r="M26" s="159"/>
       <c r="O26" s="22"/>
       <c r="S26" s="23" t="s">
         <v>48</v>
@@ -5464,19 +5216,21 @@
       </c>
     </row>
     <row r="27" spans="1:21" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="96"/>
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="97"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="97"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="97"/>
-      <c r="I27" s="97"/>
-      <c r="J27" s="97"/>
-      <c r="K27" s="97"/>
-      <c r="L27" s="97"/>
-      <c r="M27" s="98"/>
+      <c r="A27" s="149" t="s">
+        <v>498</v>
+      </c>
+      <c r="B27" s="150"/>
+      <c r="C27" s="150"/>
+      <c r="D27" s="150"/>
+      <c r="E27" s="150"/>
+      <c r="F27" s="150"/>
+      <c r="G27" s="150"/>
+      <c r="H27" s="150"/>
+      <c r="I27" s="150"/>
+      <c r="J27" s="150"/>
+      <c r="K27" s="150"/>
+      <c r="L27" s="150"/>
+      <c r="M27" s="151"/>
       <c r="O27" s="4" t="s">
         <v>1</v>
       </c>
@@ -5492,61 +5246,63 @@
       </c>
     </row>
     <row r="28" spans="1:21" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="106" t="s">
-        <v>469</v>
-      </c>
-      <c r="B28" s="107"/>
-      <c r="C28" s="107"/>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="107"/>
-      <c r="H28" s="107"/>
-      <c r="I28" s="107"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="107"/>
-      <c r="L28" s="107"/>
-      <c r="M28" s="108"/>
+      <c r="A28" s="157" t="s">
+        <v>459</v>
+      </c>
+      <c r="B28" s="158"/>
+      <c r="C28" s="158"/>
+      <c r="D28" s="158"/>
+      <c r="E28" s="158"/>
+      <c r="F28" s="158"/>
+      <c r="G28" s="158"/>
+      <c r="H28" s="158"/>
+      <c r="I28" s="158"/>
+      <c r="J28" s="158"/>
+      <c r="K28" s="158"/>
+      <c r="L28" s="158"/>
+      <c r="M28" s="159"/>
       <c r="O28" s="4"/>
       <c r="S28" s="14"/>
       <c r="T28" s="15"/>
       <c r="U28" s="11"/>
     </row>
     <row r="29" spans="1:21" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="96"/>
-      <c r="B29" s="97"/>
-      <c r="C29" s="97"/>
-      <c r="D29" s="97"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="97"/>
-      <c r="G29" s="97"/>
-      <c r="H29" s="97"/>
-      <c r="I29" s="97"/>
-      <c r="J29" s="97"/>
-      <c r="K29" s="97"/>
-      <c r="L29" s="97"/>
-      <c r="M29" s="98"/>
+      <c r="A29" s="149" t="s">
+        <v>499</v>
+      </c>
+      <c r="B29" s="150"/>
+      <c r="C29" s="150"/>
+      <c r="D29" s="150"/>
+      <c r="E29" s="150"/>
+      <c r="F29" s="150"/>
+      <c r="G29" s="150"/>
+      <c r="H29" s="150"/>
+      <c r="I29" s="150"/>
+      <c r="J29" s="150"/>
+      <c r="K29" s="150"/>
+      <c r="L29" s="150"/>
+      <c r="M29" s="151"/>
       <c r="O29" s="4"/>
       <c r="S29" s="14"/>
       <c r="T29" s="15"/>
       <c r="U29" s="11"/>
     </row>
     <row r="30" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="148" t="s">
-        <v>480</v>
-      </c>
-      <c r="B30" s="149"/>
-      <c r="C30" s="149"/>
-      <c r="D30" s="149"/>
-      <c r="E30" s="149"/>
-      <c r="F30" s="149"/>
-      <c r="G30" s="149"/>
-      <c r="H30" s="149"/>
-      <c r="I30" s="149"/>
-      <c r="J30" s="149"/>
-      <c r="K30" s="149"/>
-      <c r="L30" s="149"/>
-      <c r="M30" s="150"/>
+      <c r="A30" s="78" t="s">
+        <v>467</v>
+      </c>
+      <c r="B30" s="79"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="80"/>
       <c r="O30" s="4" t="s">
         <v>6</v>
       </c>
@@ -5555,19 +5311,19 @@
       <c r="U30" s="11"/>
     </row>
     <row r="31" spans="1:21" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="148"/>
-      <c r="B31" s="149"/>
-      <c r="C31" s="149"/>
-      <c r="D31" s="149"/>
-      <c r="E31" s="149"/>
-      <c r="F31" s="149"/>
-      <c r="G31" s="149"/>
-      <c r="H31" s="149"/>
-      <c r="I31" s="149"/>
-      <c r="J31" s="149"/>
-      <c r="K31" s="149"/>
-      <c r="L31" s="149"/>
-      <c r="M31" s="150"/>
+      <c r="A31" s="78"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="80"/>
       <c r="O31" s="4" t="s">
         <v>5</v>
       </c>
@@ -5576,19 +5332,19 @@
       <c r="U31" s="11"/>
     </row>
     <row r="32" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="148"/>
-      <c r="B32" s="149"/>
-      <c r="C32" s="149"/>
-      <c r="D32" s="149"/>
-      <c r="E32" s="149"/>
-      <c r="F32" s="149"/>
-      <c r="G32" s="149"/>
-      <c r="H32" s="149"/>
-      <c r="I32" s="149"/>
-      <c r="J32" s="149"/>
-      <c r="K32" s="149"/>
-      <c r="L32" s="149"/>
-      <c r="M32" s="150"/>
+      <c r="A32" s="78"/>
+      <c r="B32" s="79"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="79"/>
+      <c r="E32" s="79"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="79"/>
+      <c r="J32" s="79"/>
+      <c r="K32" s="79"/>
+      <c r="L32" s="79"/>
+      <c r="M32" s="80"/>
       <c r="O32" s="4" t="s">
         <v>9</v>
       </c>
@@ -5604,19 +5360,19 @@
       </c>
     </row>
     <row r="33" spans="1:21" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="148"/>
-      <c r="B33" s="149"/>
-      <c r="C33" s="149"/>
-      <c r="D33" s="149"/>
-      <c r="E33" s="149"/>
-      <c r="F33" s="149"/>
-      <c r="G33" s="149"/>
-      <c r="H33" s="149"/>
-      <c r="I33" s="149"/>
-      <c r="J33" s="149"/>
-      <c r="K33" s="149"/>
-      <c r="L33" s="149"/>
-      <c r="M33" s="150"/>
+      <c r="A33" s="78"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="79"/>
+      <c r="I33" s="79"/>
+      <c r="J33" s="79"/>
+      <c r="K33" s="79"/>
+      <c r="L33" s="79"/>
+      <c r="M33" s="80"/>
       <c r="N33" s="27"/>
       <c r="O33" s="4" t="s">
         <v>10</v>
@@ -5633,19 +5389,19 @@
       </c>
     </row>
     <row r="34" spans="1:21" s="1" customFormat="1" ht="162.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="148"/>
-      <c r="B34" s="149"/>
-      <c r="C34" s="149"/>
-      <c r="D34" s="149"/>
-      <c r="E34" s="149"/>
-      <c r="F34" s="149"/>
-      <c r="G34" s="149"/>
-      <c r="H34" s="149"/>
-      <c r="I34" s="149"/>
-      <c r="J34" s="149"/>
-      <c r="K34" s="149"/>
-      <c r="L34" s="149"/>
-      <c r="M34" s="150"/>
+      <c r="A34" s="78"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="79"/>
+      <c r="H34" s="79"/>
+      <c r="I34" s="79"/>
+      <c r="J34" s="79"/>
+      <c r="K34" s="79"/>
+      <c r="L34" s="79"/>
+      <c r="M34" s="80"/>
       <c r="N34" s="27"/>
       <c r="O34" s="4" t="s">
         <v>7</v>
@@ -5662,10 +5418,10 @@
       </c>
     </row>
     <row r="35" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="82" t="s">
-        <v>459</v>
-      </c>
-      <c r="B35" s="83"/>
+      <c r="A35" s="189" t="s">
+        <v>449</v>
+      </c>
+      <c r="B35" s="190"/>
       <c r="C35" s="51"/>
       <c r="D35" s="51"/>
       <c r="E35" s="51"/>
@@ -5673,12 +5429,12 @@
       <c r="G35" s="51"/>
       <c r="H35" s="51"/>
       <c r="I35" s="51"/>
-      <c r="J35" s="61" t="s">
-        <v>458</v>
-      </c>
-      <c r="K35" s="61"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="62"/>
+      <c r="J35" s="145" t="s">
+        <v>448</v>
+      </c>
+      <c r="K35" s="145"/>
+      <c r="L35" s="145"/>
+      <c r="M35" s="169"/>
       <c r="N35" s="27"/>
       <c r="O35" s="4"/>
       <c r="S35" s="14"/>
@@ -5686,25 +5442,25 @@
       <c r="U35" s="11"/>
     </row>
     <row r="36" spans="1:21" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="84" t="s">
-        <v>479</v>
-      </c>
-      <c r="B36" s="85"/>
-      <c r="C36" s="57" t="s">
-        <v>462</v>
-      </c>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
+      <c r="A36" s="191" t="s">
+        <v>466</v>
+      </c>
+      <c r="B36" s="192"/>
+      <c r="C36" s="166" t="s">
+        <v>452</v>
+      </c>
+      <c r="D36" s="146"/>
+      <c r="E36" s="146"/>
+      <c r="F36" s="146"/>
+      <c r="G36" s="146"/>
       <c r="H36" s="51"/>
       <c r="I36" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="J36" s="58"/>
-      <c r="K36" s="58"/>
+      <c r="J36" s="146"/>
+      <c r="K36" s="146"/>
       <c r="L36" s="51" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="M36" s="54">
         <v>2019</v>
@@ -5716,16 +5472,16 @@
       <c r="U36" s="11"/>
     </row>
     <row r="37" spans="1:21" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="59" t="s">
-        <v>464</v>
-      </c>
-      <c r="B37" s="60"/>
-      <c r="C37" s="92" t="s">
-        <v>461</v>
-      </c>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61"/>
+      <c r="A37" s="167" t="s">
+        <v>454</v>
+      </c>
+      <c r="B37" s="168"/>
+      <c r="C37" s="144" t="s">
+        <v>451</v>
+      </c>
+      <c r="D37" s="145"/>
+      <c r="E37" s="145"/>
+      <c r="F37" s="145"/>
       <c r="G37" s="51"/>
       <c r="H37" s="51"/>
       <c r="I37" s="51"/>
@@ -5757,14 +5513,14 @@
       <c r="E38" s="28"/>
       <c r="F38" s="28"/>
       <c r="G38" s="40"/>
-      <c r="H38" s="89" t="s">
+      <c r="H38" s="141" t="s">
         <v>431</v>
       </c>
-      <c r="I38" s="90"/>
-      <c r="J38" s="90"/>
-      <c r="K38" s="90"/>
-      <c r="L38" s="90"/>
-      <c r="M38" s="91"/>
+      <c r="I38" s="142"/>
+      <c r="J38" s="142"/>
+      <c r="K38" s="142"/>
+      <c r="L38" s="142"/>
+      <c r="M38" s="143"/>
       <c r="N38" s="27"/>
       <c r="O38" s="1" t="s">
         <v>433</v>
@@ -5782,25 +5538,25 @@
       </c>
     </row>
     <row r="39" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="173" t="s">
         <v>428</v>
       </c>
-      <c r="B39" s="67"/>
-      <c r="C39" s="68" t="s">
+      <c r="B39" s="174"/>
+      <c r="C39" s="175" t="s">
         <v>429</v>
       </c>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="69"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="70"/>
-      <c r="J39" s="68" t="s">
+      <c r="D39" s="176"/>
+      <c r="E39" s="176"/>
+      <c r="F39" s="176"/>
+      <c r="G39" s="176"/>
+      <c r="H39" s="176"/>
+      <c r="I39" s="177"/>
+      <c r="J39" s="175" t="s">
         <v>426</v>
       </c>
-      <c r="K39" s="69"/>
-      <c r="L39" s="69"/>
-      <c r="M39" s="70"/>
+      <c r="K39" s="176"/>
+      <c r="L39" s="176"/>
+      <c r="M39" s="177"/>
       <c r="N39" s="50"/>
       <c r="P39" s="2"/>
       <c r="S39" s="14" t="s">
@@ -5815,25 +5571,25 @@
       </c>
     </row>
     <row r="40" spans="1:21" s="1" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="71" t="s">
+      <c r="A40" s="178" t="s">
+        <v>442</v>
+      </c>
+      <c r="B40" s="179"/>
+      <c r="C40" s="180" t="s">
+        <v>460</v>
+      </c>
+      <c r="D40" s="181"/>
+      <c r="E40" s="181"/>
+      <c r="F40" s="181"/>
+      <c r="G40" s="181"/>
+      <c r="H40" s="181"/>
+      <c r="I40" s="182"/>
+      <c r="J40" s="186" t="s">
         <v>443</v>
       </c>
-      <c r="B40" s="72"/>
-      <c r="C40" s="73" t="s">
-        <v>470</v>
-      </c>
-      <c r="D40" s="74"/>
-      <c r="E40" s="74"/>
-      <c r="F40" s="74"/>
-      <c r="G40" s="74"/>
-      <c r="H40" s="74"/>
-      <c r="I40" s="75"/>
-      <c r="J40" s="79" t="s">
-        <v>444</v>
-      </c>
-      <c r="K40" s="80"/>
-      <c r="L40" s="80"/>
-      <c r="M40" s="81"/>
+      <c r="K40" s="187"/>
+      <c r="L40" s="187"/>
+      <c r="M40" s="188"/>
       <c r="N40" s="27"/>
       <c r="P40" s="2"/>
       <c r="S40" s="14" t="s">
@@ -5848,25 +5604,25 @@
       </c>
     </row>
     <row r="41" spans="1:21" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="76" t="s">
+      <c r="A41" s="183" t="s">
         <v>432</v>
       </c>
-      <c r="B41" s="77"/>
-      <c r="C41" s="76" t="s">
+      <c r="B41" s="184"/>
+      <c r="C41" s="183" t="s">
         <v>430</v>
       </c>
-      <c r="D41" s="78"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
-      <c r="H41" s="78"/>
-      <c r="I41" s="77"/>
-      <c r="J41" s="76" t="s">
+      <c r="D41" s="185"/>
+      <c r="E41" s="185"/>
+      <c r="F41" s="185"/>
+      <c r="G41" s="185"/>
+      <c r="H41" s="185"/>
+      <c r="I41" s="184"/>
+      <c r="J41" s="183" t="s">
         <v>432</v>
       </c>
-      <c r="K41" s="78"/>
-      <c r="L41" s="78"/>
-      <c r="M41" s="77"/>
+      <c r="K41" s="185"/>
+      <c r="L41" s="185"/>
+      <c r="M41" s="184"/>
       <c r="O41" s="4"/>
       <c r="P41" s="2"/>
       <c r="S41" s="14" t="s">
@@ -5908,21 +5664,21 @@
       </c>
     </row>
     <row r="43" spans="1:21" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="65" t="s">
-        <v>467</v>
-      </c>
-      <c r="B43" s="65"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="65"/>
-      <c r="G43" s="65"/>
-      <c r="H43" s="65"/>
-      <c r="I43" s="65"/>
-      <c r="J43" s="65"/>
-      <c r="K43" s="65"/>
-      <c r="L43" s="65"/>
-      <c r="M43" s="65"/>
+      <c r="A43" s="172" t="s">
+        <v>457</v>
+      </c>
+      <c r="B43" s="172"/>
+      <c r="C43" s="172"/>
+      <c r="D43" s="172"/>
+      <c r="E43" s="172"/>
+      <c r="F43" s="172"/>
+      <c r="G43" s="172"/>
+      <c r="H43" s="172"/>
+      <c r="I43" s="172"/>
+      <c r="J43" s="172"/>
+      <c r="K43" s="172"/>
+      <c r="L43" s="172"/>
+      <c r="M43" s="172"/>
       <c r="O43" s="4"/>
       <c r="P43" s="2"/>
       <c r="S43" s="14"/>
@@ -6221,7 +5977,7 @@
         <v xml:space="preserve">075 - BANCO CR2 S.A. </v>
       </c>
       <c r="AD58" s="6" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.2">
@@ -6275,7 +6031,7 @@
         <v xml:space="preserve">078 - BI-BES E.SANTO </v>
       </c>
       <c r="AD61" s="6" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.2">
@@ -6293,7 +6049,7 @@
         <v xml:space="preserve">079 - JBS BANCO S.A. </v>
       </c>
       <c r="AD62" s="6" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
@@ -6311,7 +6067,7 @@
         <v>080 - SCBT ASSOCIADOS</v>
       </c>
       <c r="AD63" s="6" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.2">
@@ -9650,16 +9406,50 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="70">
-    <mergeCell ref="A11:M11"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A20:M20"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="A18:M18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A43:M43"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:I39"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A29:M29"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="A1:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="A7:I7"/>
     <mergeCell ref="A30:M34"/>
     <mergeCell ref="C22:D23"/>
     <mergeCell ref="E22:G23"/>
@@ -9676,50 +9466,16 @@
     <mergeCell ref="H22:J22"/>
     <mergeCell ref="K22:M22"/>
     <mergeCell ref="H17:M17"/>
-    <mergeCell ref="A1:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A29:M29"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="A27:M27"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="A26:M26"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="A28:M28"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A43:M43"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:I39"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:I40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A11:M11"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A20:M20"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="A18:M18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K8">
@@ -9728,20 +9484,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="164" yWindow="725" count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Selecione uma opção:" error="POR FAVOR SOLECIONE UMA OPÇÃO!!!!" promptTitle="Selecione uma opção:" prompt="Selecione o Nível relacionado à modalidade, caso possua._x000a__x000a_" sqref="B24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Selecione uma opção:" error="POR FAVOR SOLECIONE UMA OPÇÃO!!!!" promptTitle="Selecione uma opção:" prompt="Selecione o Nível relacionado à modalidade, caso possua._x000a__x000a_" sqref="B24">
       <formula1>"***,A,B,C,D"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Selecione uma opção:" error="POR FAVOR SOLECIONE UMA OPÇÃO!!!!" promptTitle="Selecione uma opção:" prompt="Selecione a CATEGORIA da bolsa._x000a__x000a_" sqref="A22:B22" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Selecione uma opção:" error="POR FAVOR SOLECIONE UMA OPÇÃO!!!!" promptTitle="Selecione uma opção:" prompt="Selecione a CATEGORIA da bolsa._x000a__x000a_" sqref="A22:B22">
       <formula1>"***,Bolsa de Pesquisa e de Estimulo à Inovação,Bolsa de Estudo"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Valor Mensal:" prompt="Informe o valor mensal da bolsa." sqref="H24" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Selecione uma opção:" error="POR FAVOR SOLECIONE UMA OPÇÃO!!!!" promptTitle="Selecione uma opção:" prompt="Selecione a modalidade da bolsa._x000a__x000a_" sqref="A24" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Valor Mensal:" prompt="Informe o valor mensal da bolsa." sqref="H24"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Selecione uma opção:" error="POR FAVOR SOLECIONE UMA OPÇÃO!!!!" promptTitle="Selecione uma opção:" prompt="Selecione a modalidade da bolsa._x000a__x000a_" sqref="A24">
       <formula1>$AD$53:$AD$63</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Período:" prompt="Informe nº de meses." sqref="H22" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>0</formula1>
-      <formula2>99999999</formula2>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Período:" prompt="Informe nº de meses." sqref="H22:J22"/>
   </dataValidations>
   <pageMargins left="0.39370078740157483" right="0.11811023622047245" top="0.19685039370078741" bottom="0" header="0" footer="0"/>
   <pageSetup scale="80" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -9759,7 +9512,7 @@
                   <from>
                     <xdr:col>12</xdr:col>
                     <xdr:colOff>495300</xdr:colOff>
-                    <xdr:row>6</xdr:row>
+                    <xdr:row>5</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
@@ -9782,7 +9535,7 @@
                     <xdr:col>12</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>219075</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>12</xdr:col>

</xml_diff>